<commit_message>
updated data analysis again ...
</commit_message>
<xml_diff>
--- a/REyeker-DataAnalyses-Python/data/aoi_categorized/AOI_TI_IntegerBinary.xlsx
+++ b/REyeker-DataAnalyses-Python/data/aoi_categorized/AOI_TI_IntegerBinary.xlsx
@@ -404,286 +404,247 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1">
-        <v>0</v>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>33</v>
       </c>
       <c r="B2">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="C2">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>624</v>
-      </c>
-      <c r="F2" t="s">
+        <v>624</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1">
-        <v>1</v>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>61</v>
       </c>
       <c r="B3">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="C3">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>624</v>
-      </c>
-      <c r="F3" t="s">
+        <v>624</v>
+      </c>
+      <c r="E3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1">
-        <v>2</v>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>89</v>
       </c>
       <c r="B4">
-        <v>89</v>
+        <v>116</v>
       </c>
       <c r="C4">
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>624</v>
-      </c>
-      <c r="F4" t="s">
+        <v>624</v>
+      </c>
+      <c r="E4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1">
-        <v>3</v>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>117</v>
       </c>
       <c r="B5">
-        <v>117</v>
+        <v>144</v>
       </c>
       <c r="C5">
-        <v>144</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>624</v>
-      </c>
-      <c r="F5" t="s">
+        <v>624</v>
+      </c>
+      <c r="E5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1">
-        <v>4</v>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>173</v>
       </c>
       <c r="B6">
-        <v>173</v>
+        <v>200</v>
       </c>
       <c r="C6">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>624</v>
-      </c>
-      <c r="F6" t="s">
+        <v>624</v>
+      </c>
+      <c r="E6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1">
-        <v>5</v>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>201</v>
       </c>
       <c r="B7">
-        <v>201</v>
+        <v>228</v>
       </c>
       <c r="C7">
-        <v>228</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>624</v>
-      </c>
-      <c r="F7" t="s">
+        <v>624</v>
+      </c>
+      <c r="E7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1">
-        <v>6</v>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>229</v>
       </c>
       <c r="B8">
-        <v>229</v>
+        <v>256</v>
       </c>
       <c r="C8">
-        <v>256</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>624</v>
-      </c>
-      <c r="F8" t="s">
+        <v>624</v>
+      </c>
+      <c r="E8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="1">
-        <v>7</v>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>257</v>
       </c>
       <c r="B9">
-        <v>257</v>
+        <v>284</v>
       </c>
       <c r="C9">
-        <v>284</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>624</v>
-      </c>
-      <c r="F9" t="s">
+        <v>624</v>
+      </c>
+      <c r="E9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="1">
-        <v>8</v>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>285</v>
       </c>
       <c r="B10">
-        <v>285</v>
+        <v>312</v>
       </c>
       <c r="C10">
-        <v>312</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>624</v>
-      </c>
-      <c r="F10" t="s">
+        <v>624</v>
+      </c>
+      <c r="E10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="1">
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>313</v>
+      </c>
+      <c r="B11">
+        <v>340</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>624</v>
+      </c>
+      <c r="E11" t="s">
         <v>9</v>
       </c>
-      <c r="B11">
-        <v>313</v>
-      </c>
-      <c r="C11">
-        <v>340</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>624</v>
-      </c>
-      <c r="F11" t="s">
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>341</v>
+      </c>
+      <c r="B12">
+        <v>368</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>624</v>
+      </c>
+      <c r="E12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="1">
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>397</v>
+      </c>
+      <c r="B13">
+        <v>424</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>624</v>
+      </c>
+      <c r="E13" t="s">
         <v>10</v>
       </c>
-      <c r="B12">
-        <v>341</v>
-      </c>
-      <c r="C12">
-        <v>368</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>624</v>
-      </c>
-      <c r="F12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>397</v>
-      </c>
-      <c r="C13">
-        <v>424</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>624</v>
-      </c>
-      <c r="F13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="1">
-        <v>12</v>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>425</v>
       </c>
       <c r="B14">
-        <v>425</v>
+        <v>452</v>
       </c>
       <c r="C14">
-        <v>452</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>624</v>
-      </c>
-      <c r="F14" t="s">
+        <v>624</v>
+      </c>
+      <c r="E14" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>